<commit_message>
New librarian information written to shcedule file
</commit_message>
<xml_diff>
--- a/ScheduleInfo/Avvikelser schema.xlsx
+++ b/ScheduleInfo/Avvikelser schema.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Master Thesis\main\ScheduleInfo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\MasterThesis\ScheduleInfo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -264,12 +264,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE6FF00"/>
+        <bgColor rgb="FFE6FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -327,7 +339,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -338,6 +350,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -619,460 +637,579 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" style="11" customWidth="1"/>
+    <col min="2" max="2" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="5"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="D2" s="2"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2"/>
       <c r="C3" s="2"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="5"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="D3" s="2"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2"/>
       <c r="C4" s="2"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="5"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="D4" s="2"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="5"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="D5" s="2"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="5"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="D6" s="2"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="2"/>
       <c r="C7" s="2"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="D7" s="2"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="10">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="5"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="D8" s="2"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="10">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="5"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="D9" s="2"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="5"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="E10" s="4"/>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="2"/>
       <c r="C11" s="2"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="5"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="D11" s="2"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="5"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="D12" s="2"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="2"/>
       <c r="C13" s="2"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="5"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="D13" s="2"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="2"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="2"/>
+      <c r="E14" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="5"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="10">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="2"/>
+      <c r="D15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="5"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="E15" s="4"/>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="2"/>
       <c r="C16" s="2"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="5" t="s">
+      <c r="D16" s="2"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="10">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="2"/>
+      <c r="D17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="5"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="E17" s="4"/>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="10">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="E18" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E18" s="5"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="2"/>
       <c r="C19" s="2"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="5"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="D19" s="2"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="10">
+        <v>19</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="2"/>
+      <c r="D20" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="5"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="E20" s="4"/>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>20</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="2"/>
       <c r="C21" s="2"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="5"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="D21" s="2"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="10">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="2"/>
+      <c r="D22" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="5" t="s">
+      <c r="E22" s="4"/>
+      <c r="F22" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <v>22</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="5"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+      <c r="D23" s="2"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="10">
+        <v>23</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="5"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+      <c r="D24" s="2"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="10">
+        <v>24</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D25" s="4"/>
-      <c r="E25" s="5"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="E25" s="4"/>
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="10">
+        <v>25</v>
+      </c>
+      <c r="B26" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="C26" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="C26" s="2"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="5"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="D26" s="12"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="14"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>26</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="5"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+      <c r="D27" s="2"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="10">
+        <v>27</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C28" s="2"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="5"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+      <c r="D28" s="2"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>28</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C29" s="2"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="5"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+      <c r="D29" s="2"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="5"/>
+    </row>
+    <row r="30" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>29</v>
+      </c>
+      <c r="B30" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="C30" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="C30" s="2"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="5"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+      <c r="D30" s="12"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="14"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>30</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="2"/>
       <c r="C31" s="2"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="5" t="s">
+      <c r="D31" s="2"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="5" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="10">
+        <v>31</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="2"/>
+      <c r="D32" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D32" s="4"/>
-      <c r="E32" s="5"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+      <c r="E32" s="4"/>
+      <c r="F32" s="5"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="10">
+        <v>32</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="C33" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C33" s="2"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="5"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+      <c r="D33" s="2"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="5"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>33</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="C34" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C34" s="2"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="5" t="s">
+      <c r="D34" s="2"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="5" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>34</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C35" s="2"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="5"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+      <c r="D35" s="2"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="5"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>35</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="2"/>
+      <c r="D36" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="E36" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E36" s="5" t="s">
+      <c r="F36" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="10">
+        <v>36</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="C37" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C37" s="2"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="5"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
+      <c r="D37" s="2"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="5"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="10">
+        <v>37</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B38" s="2"/>
       <c r="C38" s="2"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="5"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
+      <c r="D38" s="2"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="5"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="10">
+        <v>38</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="C39" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C39" s="2"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="5"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+      <c r="D39" s="2"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="5"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>39</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="C40" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C40" s="2"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="5"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>